<commit_message>
Atualização automática de TRIUNFO.xlsx
</commit_message>
<xml_diff>
--- a/TRIUNFO.xlsx
+++ b/TRIUNFO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48A3E369-81BC-4948-B20B-10BFF9E7FF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC72754A-A130-40BD-983B-31862F95FEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1226,7 +1226,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{0C01E8BD-934F-4FA6-B1A7-BF68F2C58C54}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{CA81B95A-5E5D-4BCD-A0E8-8A76A7FDFFDE}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1256,10 +1256,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28160DC-8270-4781-BDAD-10A807C869BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34C0B51B-D560-4985-88E6-36B8CE78BCE4}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1297,7 +1297,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5B81FE9-BB63-49FF-8906-9DFA60C184D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D82557BF-1309-47F2-83F5-ABA2DD47BE33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1360,7 +1360,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75279292-449B-4710-99B4-4D2E14AD3D0C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3982AFE2-1611-451C-9D6E-EC2BAAFD6D79}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1379,7 +1379,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDFE0B3C-4014-44F1-71B4-7E15443466C8}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C8C1591-03D2-B06C-080D-FA3D3C1B1489}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1428,7 +1428,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6904B47-38EA-B56F-1DE7-039AAF80D355}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7967C472-D161-9ACC-8245-3971C430CE8B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1447,7 +1447,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43A4CDE2-54EC-2339-0117-43324F3AF765}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FD542DD-9873-FCAE-1BA3-97E650171B96}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1478,7 +1478,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97DD88A2-C2D3-1074-B3F8-0A88213EEF54}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{775CC229-7E27-32E7-5638-30FD6E75E206}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1509,7 +1509,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1B43A85-7F67-B0B6-4EDF-9736E0546BB7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FBEBBDA-8241-5210-4D72-1BB327990DBC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1552,7 +1552,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC02EF7F-A47E-4503-BB31-9B29A2FD42DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49332B39-B382-46CC-982D-940B87A32B09}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1590,7 +1590,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{400A9ACA-7DF3-4799-B36E-075EB74E4C4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{311A5B79-D0A8-41F3-B4FA-7FE1053E9632}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1633,7 +1633,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B426FEC0-E021-426F-9CE9-2950555DBC54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57DC7F35-6E47-40BF-B7E0-F0724F9C5278}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1946,7 +1946,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8974C7BD-4614-41A7-B519-68AF3E14A98C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44EAB6F3-8CEF-4CC0-9E14-0A6A8EEB9ADF}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>